<commit_message>
Actualización de imágenes en plan de implementación y carta gantt
</commit_message>
<xml_diff>
--- a/2018/bibliografia/PlanImplementacion.xlsx
+++ b/2018/bibliografia/PlanImplementacion.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mgr\UNAP Título 2018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sync\resilio.sync\pipe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635FF66A-DB39-47A3-AE8C-22BEC8A6EB49}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E06932-094F-4410-BF7A-EB902B4B356F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8925" xr2:uid="{265AA247-8EEA-45D7-A080-B942DA834545}"/>
   </bookViews>
@@ -35,9 +35,6 @@
     <t>Presentar Manual al comité de ejecutivos</t>
   </si>
   <si>
-    <t>Fecha Inicio</t>
-  </si>
-  <si>
     <t>Actividad</t>
   </si>
   <si>
@@ -95,6 +92,10 @@
   </si>
   <si>
     <t>Socializar el Manual de buenas prácticas en la Gerencia General y Gerencia Legal</t>
+  </si>
+  <si>
+    <t>Fecha 
+Inicio</t>
   </si>
 </sst>
 </file>
@@ -158,7 +159,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -227,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -244,46 +245,52 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -600,246 +607,252 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7C06B7D-D098-4138-BDAA-3A4355A157D8}">
-  <dimension ref="B3:H12"/>
+  <dimension ref="B1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="4.42578125" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.85546875" customWidth="1"/>
     <col min="3" max="3" width="50.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" style="12" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="33.140625" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
+    <row r="1" spans="2:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>43467</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="6">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="3">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="7">
+        <v>43472</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="12">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H4" s="9">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
         <v>3</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="4">
-        <v>43467</v>
-      </c>
-      <c r="E4" s="3">
-        <v>1</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="C5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="7">
+        <v>43475</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="8">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="3">
-        <v>2</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="9">
-        <v>43472</v>
-      </c>
-      <c r="E5" s="10">
-        <v>0.75</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="14">
+      <c r="G5" s="12">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="9">
         <v>0.125</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="9">
-        <v>43475</v>
-      </c>
-      <c r="E6" s="10">
+      <c r="D6" s="7">
+        <v>43480</v>
+      </c>
+      <c r="E6" s="8">
         <v>0.75</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="14">
+        <v>10</v>
+      </c>
+      <c r="G6" s="12">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="9">
         <v>0.125</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
+    <row r="7" spans="2:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="3">
+        <v>5</v>
+      </c>
       <c r="C7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="9">
-        <v>43480</v>
-      </c>
-      <c r="E7" s="10">
+        <v>16</v>
+      </c>
+      <c r="D7" s="7">
+        <v>43121</v>
+      </c>
+      <c r="E7" s="8">
         <v>0.75</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="14">
+        <v>10</v>
+      </c>
+      <c r="G7" s="12">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="9">
         <v>0.125</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
+    <row r="8" spans="2:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="3">
+        <v>6</v>
+      </c>
       <c r="C8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="9">
-        <v>43121</v>
-      </c>
-      <c r="E8" s="10">
-        <v>0.75</v>
+        <v>3</v>
+      </c>
+      <c r="D8" s="7">
+        <v>43486</v>
+      </c>
+      <c r="E8" s="8">
+        <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="14">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="H8" s="11">
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G8" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="H8" s="9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="9">
-        <v>43486</v>
-      </c>
-      <c r="E9" s="10">
-        <v>1</v>
+      <c r="D9" s="4">
+        <v>43467</v>
+      </c>
+      <c r="E9" s="3">
+        <v>3</v>
       </c>
       <c r="F9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="11">
+        <v>0.4</v>
+      </c>
+      <c r="H9" s="9">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="3">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="7">
+        <v>43493</v>
+      </c>
+      <c r="E10" s="8">
+        <v>4</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="13">
-        <v>0.25</v>
-      </c>
-      <c r="H9" s="11">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="3">
-        <v>5</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="4">
-        <v>43467</v>
-      </c>
-      <c r="E10" s="3">
-        <v>3</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="13">
-        <v>0.4</v>
-      </c>
-      <c r="H10" s="11">
-        <v>0.8</v>
+      <c r="G10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="9">
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="3">
+      <c r="B11" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="9">
-        <v>43493</v>
-      </c>
-      <c r="E11" s="10">
-        <v>4</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="10">
+      <c r="C11" s="16"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="18">
         <v>8</v>
       </c>
-      <c r="F12" s="18"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="11">
-        <f>SUM(H4:H11)</f>
+      <c r="F11" s="19"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="21">
+        <f>SUM(H3:H10)</f>
         <v>5.05</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="F11:G11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Se actualiza la valorización del plan de acción
</commit_message>
<xml_diff>
--- a/2018/bibliografia/PlanImplementacion.xlsx
+++ b/2018/bibliografia/PlanImplementacion.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sync\resilio.sync\pipe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\pCloudDrive\mauricio.camara\tituloUnap.git\2018\bibliografia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E06932-094F-4410-BF7A-EB902B4B356F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F5BF6A-7DB7-4BE6-8F97-7E1A70D1F0BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8925" xr2:uid="{265AA247-8EEA-45D7-A080-B942DA834545}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
   <si>
     <t>Presentar Manual al comité de ejecutivos</t>
   </si>
@@ -50,27 +50,13 @@
     <t>Marcha blanca del Manual de Buenas Prácticas</t>
   </si>
   <si>
-    <t>Totales</t>
-  </si>
-  <si>
     <t>Duración (semanas)</t>
   </si>
   <si>
-    <t>Costo de los Recursos (MM$)</t>
-  </si>
-  <si>
-    <t>25%
-25%</t>
-  </si>
-  <si>
     <t>Subgerente de TIC</t>
   </si>
   <si>
     <t>Jefe de Sistemas</t>
-  </si>
-  <si>
-    <t>Jefe de Sistemas
-Jefe de Fiscalización y Control</t>
   </si>
   <si>
     <t>Auditor</t>
@@ -96,16 +82,51 @@
   <si>
     <t>Fecha 
 Inicio</t>
+  </si>
+  <si>
+    <t>Jefe de Fiscalización y Control</t>
+  </si>
+  <si>
+    <t>$ Semana</t>
+  </si>
+  <si>
+    <t>Sueldo Bruto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Totales    </t>
+  </si>
+  <si>
+    <t>Rol</t>
+  </si>
+  <si>
+    <t>HH</t>
+  </si>
+  <si>
+    <t>Costo M$</t>
+  </si>
+  <si>
+    <t>$ HH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Totales   </t>
+  </si>
+  <si>
+    <t>H.H.</t>
+  </si>
+  <si>
+    <t>Costo 
+$</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0%"/>
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +164,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -164,7 +200,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -224,16 +260,100 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -245,16 +365,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -263,15 +377,25 @@
     <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -281,21 +405,107 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -607,252 +817,502 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7C06B7D-D098-4138-BDAA-3A4355A157D8}">
-  <dimension ref="B1:H11"/>
+  <dimension ref="B1:O22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" customWidth="1"/>
     <col min="3" max="3" width="50.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
     <col min="6" max="6" width="33.140625" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" style="10" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" customWidth="1"/>
+    <col min="7" max="8" width="15.140625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" customWidth="1"/>
+    <col min="12" max="12" width="28.28515625" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="13" t="s">
+    <row r="1" spans="2:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:15" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="39">
+        <v>1</v>
+      </c>
+      <c r="C3" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="37">
+        <v>43467</v>
+      </c>
+      <c r="E3" s="39">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="H3" s="2">
+        <f>41*G3*E3</f>
+        <v>10.25</v>
+      </c>
+      <c r="I3" s="48">
+        <f>ROUND(VLOOKUP($F3,$L$3:$O$6,4,FALSE)*H3,0)</f>
+        <v>150000</v>
+      </c>
+      <c r="L3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" s="14">
+        <v>2400000</v>
+      </c>
+      <c r="N3" s="15">
+        <f>ROUND(M3/4,0)</f>
+        <v>600000</v>
+      </c>
+      <c r="O3" s="15">
+        <f>N3/41</f>
+        <v>14634.146341463415</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="40"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="H4" s="2">
+        <f>41*G4*E3</f>
+        <v>10.25</v>
+      </c>
+      <c r="I4" s="48">
+        <f t="shared" ref="I4:I12" si="0">ROUND(VLOOKUP($F4,$L$3:$O$6,4,FALSE)*H4,0)</f>
+        <v>181250</v>
+      </c>
+      <c r="L4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M4" s="14">
+        <v>2900000</v>
+      </c>
+      <c r="N4" s="15">
+        <f t="shared" ref="N4:N6" si="1">ROUND(M4/4,0)</f>
+        <v>725000</v>
+      </c>
+      <c r="O4" s="15">
+        <f t="shared" ref="O4:O6" si="2">N4/41</f>
+        <v>17682.926829268294</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="5">
+        <v>43472</v>
+      </c>
+      <c r="E5" s="6">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="H5" s="34">
+        <f>E5*G5*41</f>
+        <v>10.25</v>
+      </c>
+      <c r="I5" s="48">
+        <f t="shared" si="0"/>
+        <v>237500</v>
+      </c>
+      <c r="L5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M5" s="14">
+        <v>3800000</v>
+      </c>
+      <c r="N5" s="15">
+        <f t="shared" si="1"/>
+        <v>950000</v>
+      </c>
+      <c r="O5" s="15">
+        <f t="shared" si="2"/>
+        <v>23170.731707317074</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <v>3</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="5">
+        <v>43475</v>
+      </c>
+      <c r="E6" s="6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="H6" s="34">
+        <f t="shared" ref="H6:H8" si="3">E6*G6*41</f>
+        <v>10.25</v>
+      </c>
+      <c r="I6" s="48">
+        <f t="shared" si="0"/>
+        <v>237500</v>
+      </c>
+      <c r="L6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M6" s="14">
+        <v>1800000</v>
+      </c>
+      <c r="N6" s="15">
+        <f t="shared" si="1"/>
+        <v>450000</v>
+      </c>
+      <c r="O6" s="15">
+        <f t="shared" si="2"/>
+        <v>10975.609756097561</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
+        <v>4</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="5">
+        <v>43480</v>
+      </c>
+      <c r="E7" s="6">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="H7" s="34">
+        <f t="shared" si="3"/>
+        <v>10.25</v>
+      </c>
+      <c r="I7" s="48">
+        <f t="shared" si="0"/>
+        <v>237500</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <v>5</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="5">
+        <v>43121</v>
+      </c>
+      <c r="E8" s="6">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="H8" s="34">
+        <f t="shared" si="3"/>
+        <v>10.25</v>
+      </c>
+      <c r="I8" s="48">
+        <f t="shared" si="0"/>
+        <v>237500</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="2">
+        <v>6</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="5">
+        <v>43486</v>
+      </c>
+      <c r="E9" s="6">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="H9" s="35">
+        <f>41*G9*E9</f>
+        <v>10.25</v>
+      </c>
+      <c r="I9" s="48">
+        <f t="shared" si="0"/>
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="2">
+        <v>7</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="3">
+        <v>43467</v>
+      </c>
+      <c r="E10" s="2">
+        <v>3</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="H10" s="35">
+        <f>41*G10*E10</f>
+        <v>49.2</v>
+      </c>
+      <c r="I10" s="48">
+        <f t="shared" si="0"/>
+        <v>540000</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="43">
+        <v>8</v>
+      </c>
+      <c r="C11" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="41">
+        <v>43493</v>
+      </c>
+      <c r="E11" s="46">
+        <v>4</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="H11" s="35">
+        <f>41*G11*E11</f>
+        <v>41</v>
+      </c>
+      <c r="I11" s="48">
+        <f t="shared" si="0"/>
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="44"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="45">
+        <v>0.25</v>
+      </c>
+      <c r="H12" s="36">
+        <f>41*G12*E11</f>
+        <v>41</v>
+      </c>
+      <c r="I12" s="48">
+        <f t="shared" si="0"/>
+        <v>725000</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="C13" s="19"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="11">
+        <f>SUM(E3:E11)</f>
+        <v>13</v>
+      </c>
+      <c r="F13" s="21"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="52">
+        <f>SUM(I3:I12)</f>
+        <v>3296250</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="30">
+        <v>1</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="32">
+        <f>41*25%*6</f>
+        <v>61.5</v>
+      </c>
+      <c r="E17" s="24">
+        <f>D17*O3</f>
+        <v>900000</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="30">
+        <v>2</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="32">
+        <f>41*25%*5</f>
+        <v>51.25</v>
+      </c>
+      <c r="E18" s="24">
+        <f>D18*O4</f>
+        <v>906250</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="30">
+        <v>3</v>
+      </c>
+      <c r="C19" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="4">
-        <v>43467</v>
-      </c>
-      <c r="E3" s="3">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="D19" s="32">
+        <f>41*25%*4</f>
+        <v>41</v>
+      </c>
+      <c r="E19" s="24">
+        <f>D19*O5</f>
+        <v>950000</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="31">
+        <v>4</v>
+      </c>
+      <c r="C20" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="6">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="3">
-        <v>2</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="7">
-        <v>43472</v>
-      </c>
-      <c r="E4" s="8">
-        <v>0.75</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="12">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="H4" s="9">
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="3">
-        <v>3</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="7">
-        <v>43475</v>
-      </c>
-      <c r="E5" s="8">
-        <v>0.75</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="12">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="H5" s="9">
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="3">
-        <v>4</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="7">
-        <v>43480</v>
-      </c>
-      <c r="E6" s="8">
-        <v>0.75</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="12">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="H6" s="9">
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="3">
-        <v>5</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="7">
-        <v>43121</v>
-      </c>
-      <c r="E7" s="8">
-        <v>0.75</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="12">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="H7" s="9">
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="3">
-        <v>6</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="7">
-        <v>43486</v>
-      </c>
-      <c r="E8" s="8">
-        <v>1</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="11">
-        <v>0.25</v>
-      </c>
-      <c r="H8" s="9">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="3">
-        <v>7</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="4">
-        <v>43467</v>
-      </c>
-      <c r="E9" s="3">
-        <v>3</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="11">
-        <v>0.4</v>
-      </c>
-      <c r="H9" s="9">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="3">
-        <v>8</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="7">
-        <v>43493</v>
-      </c>
-      <c r="E10" s="8">
-        <v>4</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="18">
-        <v>8</v>
-      </c>
-      <c r="F11" s="19"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="21">
-        <f>SUM(H3:H10)</f>
-        <v>5.05</v>
-      </c>
-    </row>
+      <c r="D20" s="33">
+        <f>41*G10*E10</f>
+        <v>49.2</v>
+      </c>
+      <c r="E20" s="26">
+        <f>D20*O6</f>
+        <v>540000</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="27"/>
+      <c r="C21" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="27"/>
+      <c r="E21" s="29">
+        <f>SUM(E17:E20)</f>
+        <v>3296250</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="F11:G11"/>
+  <mergeCells count="10">
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="E11:E12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Se actualizan las tablas del plan de acción
</commit_message>
<xml_diff>
--- a/2018/bibliografia/PlanImplementacion.xlsx
+++ b/2018/bibliografia/PlanImplementacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\pCloudDrive\mauricio.camara\tituloUnap.git\2018\bibliografia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F5BF6A-7DB7-4BE6-8F97-7E1A70D1F0BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4306E330-33E9-4546-A31C-C26B12F730E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8925" xr2:uid="{265AA247-8EEA-45D7-A080-B942DA834545}"/>
   </bookViews>
@@ -59,9 +59,6 @@
     <t>Jefe de Sistemas</t>
   </si>
   <si>
-    <t>Auditor</t>
-  </si>
-  <si>
     <t>Dedicación</t>
   </si>
   <si>
@@ -116,6 +113,9 @@
   <si>
     <t>Costo 
 $</t>
+  </si>
+  <si>
+    <t>Subgerente de Auditoría</t>
   </si>
 </sst>
 </file>
@@ -396,6 +396,60 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -408,50 +462,8 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -460,6 +472,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -477,28 +495,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -819,8 +819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7C06B7D-D098-4138-BDAA-3A4355A157D8}">
   <dimension ref="B1:O22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -839,51 +839,51 @@
   <sheetData>
     <row r="1" spans="2:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:15" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="18" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="10" t="s">
-        <v>27</v>
-      </c>
       <c r="M2" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N2" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O2" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="2:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="39">
+      <c r="B3" s="45">
         <v>1</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="37">
+      <c r="D3" s="41">
         <v>43467</v>
       </c>
-      <c r="E3" s="39">
+      <c r="E3" s="45">
         <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -896,7 +896,7 @@
         <f>41*G3*E3</f>
         <v>10.25</v>
       </c>
-      <c r="I3" s="48">
+      <c r="I3" s="34">
         <f>ROUND(VLOOKUP($F3,$L$3:$O$6,4,FALSE)*H3,0)</f>
         <v>150000</v>
       </c>
@@ -916,12 +916,12 @@
       </c>
     </row>
     <row r="4" spans="2:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="40"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="40"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="46"/>
       <c r="F4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G4" s="8">
         <v>0.25</v>
@@ -930,12 +930,12 @@
         <f>41*G4*E3</f>
         <v>10.25</v>
       </c>
-      <c r="I4" s="48">
+      <c r="I4" s="34">
         <f t="shared" ref="I4:I12" si="0">ROUND(VLOOKUP($F4,$L$3:$O$6,4,FALSE)*H4,0)</f>
         <v>181250</v>
       </c>
       <c r="L4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M4" s="14">
         <v>2900000</v>
@@ -954,7 +954,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="5">
         <v>43472</v>
@@ -968,11 +968,11 @@
       <c r="G5" s="13">
         <v>0.25</v>
       </c>
-      <c r="H5" s="34">
+      <c r="H5" s="30">
         <f>E5*G5*41</f>
         <v>10.25</v>
       </c>
-      <c r="I5" s="48">
+      <c r="I5" s="34">
         <f t="shared" si="0"/>
         <v>237500</v>
       </c>
@@ -996,7 +996,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="5">
         <v>43475</v>
@@ -1010,27 +1010,27 @@
       <c r="G6" s="13">
         <v>0.25</v>
       </c>
-      <c r="H6" s="34">
+      <c r="H6" s="30">
         <f t="shared" ref="H6:H8" si="3">E6*G6*41</f>
         <v>10.25</v>
       </c>
-      <c r="I6" s="48">
+      <c r="I6" s="34">
         <f t="shared" si="0"/>
         <v>237500</v>
       </c>
       <c r="L6" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="M6" s="14">
-        <v>1800000</v>
+        <v>3800000</v>
       </c>
       <c r="N6" s="15">
         <f t="shared" si="1"/>
-        <v>450000</v>
+        <v>950000</v>
       </c>
       <c r="O6" s="15">
         <f t="shared" si="2"/>
-        <v>10975.609756097561</v>
+        <v>23170.731707317074</v>
       </c>
     </row>
     <row r="7" spans="2:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -1038,7 +1038,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="5">
         <v>43480</v>
@@ -1052,11 +1052,11 @@
       <c r="G7" s="13">
         <v>0.25</v>
       </c>
-      <c r="H7" s="34">
+      <c r="H7" s="30">
         <f t="shared" si="3"/>
         <v>10.25</v>
       </c>
-      <c r="I7" s="48">
+      <c r="I7" s="34">
         <f t="shared" si="0"/>
         <v>237500</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8" s="5">
         <v>43121</v>
@@ -1080,11 +1080,11 @@
       <c r="G8" s="13">
         <v>0.25</v>
       </c>
-      <c r="H8" s="34">
+      <c r="H8" s="30">
         <f t="shared" si="3"/>
         <v>10.25</v>
       </c>
-      <c r="I8" s="48">
+      <c r="I8" s="34">
         <f t="shared" si="0"/>
         <v>237500</v>
       </c>
@@ -1108,11 +1108,11 @@
       <c r="G9" s="8">
         <v>0.25</v>
       </c>
-      <c r="H9" s="35">
+      <c r="H9" s="31">
         <f>41*G9*E9</f>
         <v>10.25</v>
       </c>
-      <c r="I9" s="48">
+      <c r="I9" s="34">
         <f t="shared" si="0"/>
         <v>150000</v>
       </c>
@@ -1131,31 +1131,31 @@
         <v>3</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="G10" s="8">
-        <v>0.4</v>
-      </c>
-      <c r="H10" s="35">
+        <v>0.3</v>
+      </c>
+      <c r="H10" s="31">
         <f>41*G10*E10</f>
-        <v>49.2</v>
-      </c>
-      <c r="I10" s="48">
-        <f t="shared" si="0"/>
-        <v>540000</v>
+        <v>36.9</v>
+      </c>
+      <c r="I10" s="34">
+        <f>ROUND(VLOOKUP($F10,$L$3:$O$6,4,FALSE)*H10,0)</f>
+        <v>855000</v>
       </c>
     </row>
     <row r="11" spans="2:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="43">
+      <c r="B11" s="49">
         <v>8</v>
       </c>
-      <c r="C11" s="50" t="s">
+      <c r="C11" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="41">
+      <c r="D11" s="47">
         <v>43493</v>
       </c>
-      <c r="E11" s="46">
+      <c r="E11" s="51">
         <v>4</v>
       </c>
       <c r="F11" s="1" t="s">
@@ -1164,140 +1164,140 @@
       <c r="G11" s="8">
         <v>0.25</v>
       </c>
-      <c r="H11" s="35">
+      <c r="H11" s="31">
         <f>41*G11*E11</f>
         <v>41</v>
       </c>
-      <c r="I11" s="48">
+      <c r="I11" s="34">
         <f t="shared" si="0"/>
         <v>600000</v>
       </c>
     </row>
     <row r="12" spans="2:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="44"/>
-      <c r="C12" s="51"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="47"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="52"/>
       <c r="F12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="45">
+        <v>16</v>
+      </c>
+      <c r="G12" s="33">
         <v>0.25</v>
       </c>
-      <c r="H12" s="36">
+      <c r="H12" s="32">
         <f>41*G12*E11</f>
         <v>41</v>
       </c>
-      <c r="I12" s="48">
+      <c r="I12" s="34">
         <f t="shared" si="0"/>
         <v>725000</v>
       </c>
     </row>
     <row r="13" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="20"/>
+      <c r="B13" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="37"/>
+      <c r="D13" s="38"/>
       <c r="E13" s="11">
         <f>SUM(E3:E11)</f>
         <v>13</v>
       </c>
-      <c r="F13" s="21"/>
-      <c r="G13" s="49"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="40"/>
       <c r="H13" s="12"/>
-      <c r="I13" s="52">
+      <c r="I13" s="35">
         <f>SUM(I3:I12)</f>
-        <v>3296250</v>
+        <v>3611250</v>
       </c>
     </row>
     <row r="16" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="18" t="s">
         <v>2</v>
       </c>
       <c r="C16" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="E16" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="22" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="17" spans="2:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="30">
+      <c r="B17" s="26">
         <v>1</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="32">
+      <c r="D17" s="28">
         <f>41*25%*6</f>
         <v>61.5</v>
       </c>
-      <c r="E17" s="24">
+      <c r="E17" s="20">
         <f>D17*O3</f>
         <v>900000</v>
       </c>
     </row>
     <row r="18" spans="2:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="30">
+      <c r="B18" s="26">
         <v>2</v>
       </c>
-      <c r="C18" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="32">
+      <c r="C18" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="28">
         <f>41*25%*5</f>
         <v>51.25</v>
       </c>
-      <c r="E18" s="24">
+      <c r="E18" s="20">
         <f>D18*O4</f>
         <v>906250</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="30">
+      <c r="B19" s="26">
         <v>3</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="32">
+      <c r="D19" s="28">
         <f>41*25%*4</f>
         <v>41</v>
       </c>
-      <c r="E19" s="24">
+      <c r="E19" s="20">
         <f>D19*O5</f>
         <v>950000</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="31">
+      <c r="B20" s="27">
         <v>4</v>
       </c>
-      <c r="C20" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="33">
+      <c r="C20" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="29">
         <f>41*G10*E10</f>
-        <v>49.2</v>
-      </c>
-      <c r="E20" s="26">
+        <v>36.9</v>
+      </c>
+      <c r="E20" s="22">
         <f>D20*O6</f>
-        <v>540000</v>
+        <v>855000</v>
       </c>
     </row>
     <row r="21" spans="2:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="27"/>
-      <c r="C21" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" s="27"/>
-      <c r="E21" s="29">
+      <c r="B21" s="23"/>
+      <c r="C21" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="23"/>
+      <c r="E21" s="25">
         <f>SUM(E17:E20)</f>
-        <v>3296250</v>
+        <v>3611250</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Versión completa de la Memoria
</commit_message>
<xml_diff>
--- a/2018/bibliografia/PlanImplementacion.xlsx
+++ b/2018/bibliografia/PlanImplementacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\pCloudDrive\mauricio.camara\tituloUnap.git\2018\bibliografia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4306E330-33E9-4546-A31C-C26B12F730E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FA4C7EB-F0A9-4EE2-A96E-AB8A26C9DC73}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8925" xr2:uid="{265AA247-8EEA-45D7-A080-B942DA834545}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
   <si>
     <t>Presentar Manual al comité de ejecutivos</t>
   </si>
@@ -90,9 +90,6 @@
     <t>Sueldo Bruto</t>
   </si>
   <si>
-    <t xml:space="preserve">Totales    </t>
-  </si>
-  <si>
     <t>Rol</t>
   </si>
   <si>
@@ -103,9 +100,6 @@
   </si>
   <si>
     <t>$ HH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Totales   </t>
   </si>
   <si>
     <t>H.H.</t>
@@ -116,6 +110,12 @@
   </si>
   <si>
     <t>Subgerente de Auditoría</t>
+  </si>
+  <si>
+    <t>TOTALES</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (suma actividades 1, 2, 3, 4, 5, 6 y 8)</t>
   </si>
 </sst>
 </file>
@@ -126,7 +126,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,6 +179,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -459,12 +466,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -500,6 +501,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -819,8 +826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7C06B7D-D098-4138-BDAA-3A4355A157D8}">
   <dimension ref="B1:O22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,10 +865,10 @@
         <v>9</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M2" s="16" t="s">
         <v>18</v>
@@ -870,20 +877,20 @@
         <v>17</v>
       </c>
       <c r="O2" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="2:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="45">
+      <c r="B3" s="43">
         <v>1</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="41">
+      <c r="D3" s="39">
         <v>43467</v>
       </c>
-      <c r="E3" s="45">
+      <c r="E3" s="43">
         <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -916,10 +923,10 @@
       </c>
     </row>
     <row r="4" spans="2:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="46"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="46"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="44"/>
       <c r="F4" s="1" t="s">
         <v>16</v>
       </c>
@@ -999,7 +1006,7 @@
         <v>12</v>
       </c>
       <c r="D6" s="5">
-        <v>43475</v>
+        <v>43479</v>
       </c>
       <c r="E6" s="6">
         <v>1</v>
@@ -1019,7 +1026,7 @@
         <v>237500</v>
       </c>
       <c r="L6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M6" s="14">
         <v>3800000</v>
@@ -1041,7 +1048,7 @@
         <v>13</v>
       </c>
       <c r="D7" s="5">
-        <v>43480</v>
+        <v>43486</v>
       </c>
       <c r="E7" s="6">
         <v>1</v>
@@ -1069,7 +1076,7 @@
         <v>11</v>
       </c>
       <c r="D8" s="5">
-        <v>43121</v>
+        <v>43493</v>
       </c>
       <c r="E8" s="6">
         <v>1</v>
@@ -1097,7 +1104,7 @@
         <v>3</v>
       </c>
       <c r="D9" s="5">
-        <v>43486</v>
+        <v>43500</v>
       </c>
       <c r="E9" s="6">
         <v>1</v>
@@ -1131,7 +1138,7 @@
         <v>3</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G10" s="8">
         <v>0.3</v>
@@ -1146,16 +1153,16 @@
       </c>
     </row>
     <row r="11" spans="2:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="49">
+      <c r="B11" s="47">
         <v>8</v>
       </c>
-      <c r="C11" s="43" t="s">
+      <c r="C11" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="47">
-        <v>43493</v>
-      </c>
-      <c r="E11" s="51">
+      <c r="D11" s="45">
+        <v>43507</v>
+      </c>
+      <c r="E11" s="49">
         <v>4</v>
       </c>
       <c r="F11" s="1" t="s">
@@ -1174,10 +1181,10 @@
       </c>
     </row>
     <row r="12" spans="2:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="50"/>
-      <c r="C12" s="44"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="52"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="50"/>
       <c r="F12" s="1" t="s">
         <v>16</v>
       </c>
@@ -1195,16 +1202,17 @@
     </row>
     <row r="13" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="36" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C13" s="37"/>
       <c r="D13" s="38"/>
       <c r="E13" s="11">
-        <f>SUM(E3:E11)</f>
-        <v>13</v>
-      </c>
-      <c r="F13" s="39"/>
-      <c r="G13" s="40"/>
+        <v>10</v>
+      </c>
+      <c r="F13" s="51" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="52"/>
       <c r="H13" s="12"/>
       <c r="I13" s="35">
         <f>SUM(I3:I12)</f>
@@ -1216,13 +1224,13 @@
         <v>2</v>
       </c>
       <c r="C16" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="E16" s="18" t="s">
         <v>21</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -1278,7 +1286,7 @@
         <v>4</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D20" s="29">
         <f>41*G10*E10</f>
@@ -1292,7 +1300,7 @@
     <row r="21" spans="2:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="23"/>
       <c r="C21" s="24" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D21" s="23"/>
       <c r="E21" s="25">

</xml_diff>